<commit_message>
Output merged excel sheet
</commit_message>
<xml_diff>
--- a/datasets/Production Oct 2023.xlsx
+++ b/datasets/Production Oct 2023.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://my.shell.com/personal/o_dejong_shell_com/Documents/Ollie de Jong/Documents/Ollie Misc/Manager stuff/New hire/Python task/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/74db7c87a9029f2a/Documents/Repos/production-data-assessment/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_19E554CD1927FD753C272A11D20D27CF6590FACE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3EB52F4-4DE7-4D72-AFE6-23D4180DFFD5}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_19E554CD1927FD753C272A11D20D27CF6590FACE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4664D222-50A3-4A64-B2F3-E8E028C98D5C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="300" yWindow="72" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,27 +375,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="37.21875" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45200</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -406,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45200</v>
       </c>
@@ -417,7 +417,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45201</v>
       </c>
@@ -428,7 +428,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45202</v>
       </c>
@@ -439,7 +439,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45203</v>
       </c>
@@ -450,7 +450,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45204</v>
       </c>
@@ -461,7 +461,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45205</v>
       </c>
@@ -472,7 +472,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45206</v>
       </c>
@@ -483,7 +483,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45207</v>
       </c>
@@ -494,7 +494,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45208</v>
       </c>
@@ -505,7 +505,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45209</v>
       </c>
@@ -516,7 +516,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45210</v>
       </c>
@@ -527,7 +527,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45211</v>
       </c>
@@ -538,7 +538,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45212</v>
       </c>
@@ -549,7 +549,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45213</v>
       </c>
@@ -560,7 +560,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45214</v>
       </c>
@@ -571,7 +571,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45215</v>
       </c>
@@ -582,7 +582,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45216</v>
       </c>
@@ -593,7 +593,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45217</v>
       </c>
@@ -604,7 +604,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45218</v>
       </c>
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45219</v>
       </c>
@@ -626,7 +626,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45220</v>
       </c>
@@ -637,7 +637,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45221</v>
       </c>
@@ -648,7 +648,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45222</v>
       </c>
@@ -659,7 +659,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45223</v>
       </c>
@@ -670,7 +670,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45224</v>
       </c>
@@ -681,7 +681,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45225</v>
       </c>
@@ -692,7 +692,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45226</v>
       </c>
@@ -703,7 +703,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45227</v>
       </c>
@@ -714,7 +714,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45228</v>
       </c>
@@ -725,7 +725,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45229</v>
       </c>
@@ -736,7 +736,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45230</v>
       </c>

</xml_diff>